<commit_message>
Update - bug fixes
</commit_message>
<xml_diff>
--- a/api/_files/CoachingSpreadsheet.xlsx
+++ b/api/_files/CoachingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Enrollees" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -70,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -91,6 +92,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -243,10 +245,10 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>

</xml_diff>

<commit_message>
Update - add sales person column
</commit_message>
<xml_diff>
--- a/api/_files/CoachingSpreadsheet.xlsx
+++ b/api/_files/CoachingSpreadsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Coach</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Person</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -236,10 +239,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,8 +255,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="57.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="57.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,6 +274,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -305,10 +310,13 @@
       <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="C1:L1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>